<commit_message>
Change state names in create_states() to be consistent across 3 and 4 state models. Ensure tutorial runs correctly with both 3 and 4 state model
</commit_message>
<xml_diff>
--- a/data-raw/utility.xlsx
+++ b/data-raw/utility.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27729"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14500" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14500" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="state_utility" sheetId="1" r:id="rId1"/>
@@ -37,79 +37,79 @@
     <t>S1</t>
   </si>
   <si>
+    <t>P2</t>
+  </si>
+  <si>
+    <t>nafees2008health</t>
+  </si>
+  <si>
+    <t>ae_name</t>
+  </si>
+  <si>
+    <t>ae_abb</t>
+  </si>
+  <si>
+    <t>Elevated alanine transaminase</t>
+  </si>
+  <si>
+    <t>alt</t>
+  </si>
+  <si>
+    <t>ast</t>
+  </si>
+  <si>
+    <t>Elevated aspartate transaminase</t>
+  </si>
+  <si>
+    <t>Diarrhea</t>
+  </si>
+  <si>
+    <t>diarrhea</t>
+  </si>
+  <si>
+    <t>Dry skin</t>
+  </si>
+  <si>
+    <t>Eye problems</t>
+  </si>
+  <si>
+    <t>Paronychia</t>
+  </si>
+  <si>
+    <t>Pneumonitis</t>
+  </si>
+  <si>
+    <t>Pruritus</t>
+  </si>
+  <si>
+    <t>Rash</t>
+  </si>
+  <si>
+    <t>Stomatitis</t>
+  </si>
+  <si>
+    <t>dry_skin</t>
+  </si>
+  <si>
+    <t>eye_problems</t>
+  </si>
+  <si>
+    <t>paronychia</t>
+  </si>
+  <si>
+    <t>pneumonitis</t>
+  </si>
+  <si>
+    <t>pruritus</t>
+  </si>
+  <si>
+    <t>rash</t>
+  </si>
+  <si>
+    <t>stomatitis</t>
+  </si>
+  <si>
     <t>P1/S2</t>
-  </si>
-  <si>
-    <t>P2</t>
-  </si>
-  <si>
-    <t>nafees2008health</t>
-  </si>
-  <si>
-    <t>ae_name</t>
-  </si>
-  <si>
-    <t>ae_abb</t>
-  </si>
-  <si>
-    <t>Elevated alanine transaminase</t>
-  </si>
-  <si>
-    <t>alt</t>
-  </si>
-  <si>
-    <t>ast</t>
-  </si>
-  <si>
-    <t>Elevated aspartate transaminase</t>
-  </si>
-  <si>
-    <t>Diarrhea</t>
-  </si>
-  <si>
-    <t>diarrhea</t>
-  </si>
-  <si>
-    <t>Dry skin</t>
-  </si>
-  <si>
-    <t>Eye problems</t>
-  </si>
-  <si>
-    <t>Paronychia</t>
-  </si>
-  <si>
-    <t>Pneumonitis</t>
-  </si>
-  <si>
-    <t>Pruritus</t>
-  </si>
-  <si>
-    <t>Rash</t>
-  </si>
-  <si>
-    <t>Stomatitis</t>
-  </si>
-  <si>
-    <t>dry_skin</t>
-  </si>
-  <si>
-    <t>eye_problems</t>
-  </si>
-  <si>
-    <t>paronychia</t>
-  </si>
-  <si>
-    <t>pneumonitis</t>
-  </si>
-  <si>
-    <t>pruritus</t>
-  </si>
-  <si>
-    <t>rash</t>
-  </si>
-  <si>
-    <t>stomatitis</t>
   </si>
 </sst>
 </file>
@@ -504,8 +504,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -540,7 +540,7 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>29</v>
       </c>
       <c r="B3">
         <v>0.6532</v>
@@ -549,12 +549,12 @@
         <v>2.223E-2</v>
       </c>
       <c r="D3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4">
         <f>B3-0.1798</f>
@@ -565,7 +565,7 @@
         <v>3.1058477103682983E-2</v>
       </c>
       <c r="D4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -582,7 +582,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
@@ -593,10 +593,10 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
         <v>8</v>
-      </c>
-      <c r="B1" t="s">
-        <v>9</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -610,10 +610,10 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
         <v>10</v>
-      </c>
-      <c r="B2" t="s">
-        <v>11</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -624,10 +624,10 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -638,10 +638,10 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
         <v>14</v>
-      </c>
-      <c r="B4" t="s">
-        <v>15</v>
       </c>
       <c r="C4">
         <v>4.6800000000000001E-2</v>
@@ -650,15 +650,15 @@
         <v>1.553E-2</v>
       </c>
       <c r="E4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -669,10 +669,10 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -683,10 +683,10 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C7">
         <v>0</v>
@@ -697,10 +697,10 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C8">
         <v>0</v>
@@ -711,10 +711,10 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C9">
         <v>0</v>
@@ -725,10 +725,10 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C10">
         <v>3.2480000000000002E-2</v>
@@ -737,15 +737,15 @@
         <v>1.171E-2</v>
       </c>
       <c r="E10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C11">
         <v>0</v>

</xml_diff>

<commit_message>
Updated utility and disutility data
</commit_message>
<xml_diff>
--- a/data-raw/utility.xlsx
+++ b/data-raw/utility.xlsx
@@ -1,16 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27729"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11110"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeroenjansen/Egnyte/Shared/RW GENERAL (MANAGEMENT)/Jeroen only access/IVI/GitHub/IVI-NSCLC/data-raw/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C56B7A1C-3652-4F49-94A1-964551E39E27}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14500" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="8000" yWindow="3040" windowWidth="25600" windowHeight="14500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="state_utility" sheetId="1" r:id="rId1"/>
     <sheet name="ae_disutility" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -118,26 +124,26 @@
     <t>notes</t>
   </si>
   <si>
-    <t>Assumed equal to rash disutility</t>
-  </si>
-  <si>
-    <t>Assumed equal to hair loss</t>
-  </si>
-  <si>
-    <t>Assumed to dyspnea</t>
-  </si>
-  <si>
-    <t>Assumed equal to fatigue disutility</t>
-  </si>
-  <si>
     <t>doyle2008health</t>
+  </si>
+  <si>
+    <t>Assumed equal to fatigue disutility; se assumed 1/3rd of mean</t>
+  </si>
+  <si>
+    <t>Assumed equal to rash disutility; se assumed 1/3rd of mean</t>
+  </si>
+  <si>
+    <t>Assumed equal to hair loss; se assumed 1/3rd of mean</t>
+  </si>
+  <si>
+    <t>Assumed equal to cough, dyspnea, and pain; se assumed 1/3rd of mean</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -157,6 +163,13 @@
       <u/>
       <sz val="12"/>
       <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -222,12 +235,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="35">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -268,6 +282,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -592,19 +614,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="4" max="4" width="15.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -618,7 +640,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -632,7 +654,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>29</v>
       </c>
@@ -646,7 +668,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -673,20 +695,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="26" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -706,7 +728,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>9</v>
       </c>
@@ -714,19 +736,21 @@
         <v>10</v>
       </c>
       <c r="C2" s="3">
-        <v>7.3459999999999998E-2</v>
+        <f>0.754-0.46</f>
+        <v>0.29399999999999998</v>
       </c>
       <c r="D2" s="3">
-        <v>1.8489999999999999E-2</v>
+        <f>ROUND(0.33*C2,3)</f>
+        <v>9.7000000000000003E-2</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>12</v>
       </c>
@@ -734,19 +758,21 @@
         <v>11</v>
       </c>
       <c r="C3" s="3">
-        <v>7.3459999999999998E-2</v>
+        <f>0.754-0.46</f>
+        <v>0.29399999999999998</v>
       </c>
       <c r="D3" s="3">
-        <v>1.8489999999999999E-2</v>
+        <f t="shared" ref="D3:D11" si="0">ROUND(0.33*C3,3)</f>
+        <v>9.7000000000000003E-2</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>13</v>
       </c>
@@ -754,56 +780,62 @@
         <v>14</v>
       </c>
       <c r="C4" s="3">
-        <v>4.6800000000000001E-2</v>
+        <f>0.754-0.532</f>
+        <v>0.22199999999999998</v>
       </c>
       <c r="D4" s="3">
-        <v>1.553E-2</v>
+        <f t="shared" si="0"/>
+        <v>7.2999999999999995E-2</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="3">
-        <v>3.2480000000000002E-2</v>
+      <c r="C5" s="1">
+        <f>0.754-0.603</f>
+        <v>0.15100000000000002</v>
       </c>
       <c r="D5" s="3">
-        <v>1.171E-2</v>
+        <f t="shared" si="0"/>
+        <v>0.05</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="3">
-        <v>4.4949999999999997E-2</v>
+      <c r="C6" s="1">
+        <f>0.754-0.616</f>
+        <v>0.13800000000000001</v>
       </c>
       <c r="D6" s="3">
-        <v>1.482E-2</v>
+        <f t="shared" si="0"/>
+        <v>4.5999999999999999E-2</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>17</v>
       </c>
@@ -811,40 +843,44 @@
         <v>24</v>
       </c>
       <c r="C7" s="1">
-        <v>3.2480000000000002E-2</v>
-      </c>
-      <c r="D7" s="1">
-        <v>1.171E-2</v>
+        <f>0.754-0.603</f>
+        <v>0.15100000000000002</v>
+      </c>
+      <c r="D7" s="3">
+        <f t="shared" si="0"/>
+        <v>0.05</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="3">
-        <v>0.05</v>
+      <c r="C8" s="1">
+        <f>0.626-0.461</f>
+        <v>0.16499999999999998</v>
       </c>
       <c r="D8" s="3">
-        <v>1.2E-2</v>
+        <f t="shared" si="0"/>
+        <v>5.3999999999999999E-2</v>
       </c>
       <c r="E8" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F8" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="F8" s="3" t="s">
-        <v>34</v>
-      </c>
       <c r="G8" s="4"/>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>19</v>
       </c>
@@ -852,19 +888,21 @@
         <v>26</v>
       </c>
       <c r="C9" s="1">
-        <v>3.2480000000000002E-2</v>
-      </c>
-      <c r="D9" s="1">
-        <v>1.171E-2</v>
+        <f>0.754-0.603</f>
+        <v>0.15100000000000002</v>
+      </c>
+      <c r="D9" s="3">
+        <f t="shared" si="0"/>
+        <v>0.05</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>20</v>
       </c>
@@ -872,16 +910,18 @@
         <v>27</v>
       </c>
       <c r="C10" s="1">
-        <v>3.2480000000000002E-2</v>
-      </c>
-      <c r="D10" s="1">
-        <v>1.171E-2</v>
+        <f>0.754-0.603</f>
+        <v>0.15100000000000002</v>
+      </c>
+      <c r="D10" s="3">
+        <f t="shared" si="0"/>
+        <v>0.05</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>21</v>
       </c>
@@ -889,16 +929,18 @@
         <v>28</v>
       </c>
       <c r="C11" s="1">
-        <v>3.2480000000000002E-2</v>
-      </c>
-      <c r="D11" s="1">
-        <v>1.171E-2</v>
+        <f>0.754-0.603</f>
+        <v>0.15100000000000002</v>
+      </c>
+      <c r="D11" s="3">
+        <f t="shared" si="0"/>
+        <v>0.05</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update R package and PDF model documentation
</commit_message>
<xml_diff>
--- a/data-raw/utility.xlsx
+++ b/data-raw/utility.xlsx
@@ -1,22 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11110"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27729"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeroenjansen/Egnyte/Shared/RW GENERAL (MANAGEMENT)/Jeroen only access/IVI/GitHub/IVI-NSCLC/data-raw/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84B07099-8149-0646-A3B3-9AAD25863CB7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8000" yWindow="3020" windowWidth="25600" windowHeight="14500" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="13940" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="state_utility" sheetId="1" r:id="rId1"/>
     <sheet name="ae_disutility" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -142,7 +136,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -614,19 +608,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="4" max="4" width="15.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -640,7 +634,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -654,7 +648,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4">
       <c r="A3" s="1" t="s">
         <v>29</v>
       </c>
@@ -668,7 +662,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -695,20 +689,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="26" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -728,7 +722,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7">
       <c r="A2" s="3" t="s">
         <v>9</v>
       </c>
@@ -739,14 +733,14 @@
         <v>0</v>
       </c>
       <c r="D2" s="3">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="5" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7">
       <c r="A3" s="3" t="s">
         <v>12</v>
       </c>
@@ -757,14 +751,14 @@
         <v>0</v>
       </c>
       <c r="D3" s="3">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="5" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7">
       <c r="A4" s="3" t="s">
         <v>13</v>
       </c>
@@ -776,14 +770,14 @@
         <v>0.22199999999999998</v>
       </c>
       <c r="D4" s="3">
-        <f t="shared" ref="D3:D11" si="0">ROUND(0.33*C4,3)</f>
+        <f t="shared" ref="D4:D11" si="0">ROUND(0.33*C4,3)</f>
         <v>7.2999999999999995E-2</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7">
       <c r="A5" s="3" t="s">
         <v>15</v>
       </c>
@@ -805,7 +799,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7">
       <c r="A6" s="3" t="s">
         <v>16</v>
       </c>
@@ -827,7 +821,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7">
       <c r="A7" s="1" t="s">
         <v>17</v>
       </c>
@@ -849,7 +843,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7">
       <c r="A8" s="3" t="s">
         <v>18</v>
       </c>
@@ -872,7 +866,7 @@
       </c>
       <c r="G8" s="4"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7">
       <c r="A9" s="1" t="s">
         <v>19</v>
       </c>
@@ -894,7 +888,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7">
       <c r="A10" s="1" t="s">
         <v>20</v>
       </c>
@@ -913,7 +907,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7">
       <c r="A11" s="1" t="s">
         <v>21</v>
       </c>

</xml_diff>